<commit_message>
Fin de la création du script d'insertion
</commit_message>
<xml_diff>
--- a/Fichiers modifiables/DonnéesExcel/ListeEspèces.xlsx
+++ b/Fichiers modifiables/DonnéesExcel/ListeEspèces.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paola.costa\Documents\GitHub\Ma-08_Zoo\Fichiers modifiables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Trimestre 6\MA 08 - Serveur BD\Ma-08_Zoo\Fichiers modifiables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>name</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>Crapeau du wioming</t>
+  </si>
+  <si>
+    <t>Gecko léopard</t>
   </si>
 </sst>
 </file>
@@ -602,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,13 +1082,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="B43">
         <v>8</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1173,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="C51">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1184,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="C52">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1195,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="C53">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1206,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="C54">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1217,224 +1220,224 @@
         <v>1</v>
       </c>
       <c r="C55">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="B56">
         <v>1</v>
       </c>
       <c r="C56">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>1</v>
       </c>
       <c r="C59">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C61">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C64">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B65">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C65">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B66">
         <v>9</v>
       </c>
       <c r="C66">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B67">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C67">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B68">
         <v>7</v>
       </c>
       <c r="C68">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C69">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B70">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C70">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C72">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C73">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74">
         <v>10</v>
       </c>
       <c r="C74">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B75">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C75">
         <v>2</v>
@@ -1442,10 +1445,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B76">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C76">
         <v>2</v>
@@ -1453,10 +1456,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B77">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C77">
         <v>2</v>
@@ -1464,10 +1467,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B78">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C78">
         <v>2</v>
@@ -1475,32 +1478,32 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B79">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B80">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C80">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C81">
         <v>2</v>
@@ -1508,23 +1511,12 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B82">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C82">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>82</v>
-      </c>
-      <c r="B83">
-        <v>6</v>
-      </c>
-      <c r="C83">
         <v>2</v>
       </c>
     </row>

</xml_diff>